<commit_message>
confirming successful development of unique ticker symbols list df this time without issues
</commit_message>
<xml_diff>
--- a/positive_yearly_earnings_per_share_2016_df.xlsx
+++ b/positive_yearly_earnings_per_share_2016_df.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25ac2033dcfcea55/Desktop/ALIENWARE - 2023-04_24 - Onwards/Python/Stock Market Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_23F921ED284B8D427A309C9F6C8A14E26E90BEA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34D0102C-2567-457D-8DB7-2B9E42B3EBB4}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -337,8 +331,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,11 +390,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -408,21 +403,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -460,7 +447,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -494,7 +481,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -529,10 +515,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -705,20 +690,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -726,819 +705,819 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>6.45</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>8.35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>6.73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>0.96</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>1.56</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>2.92</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>3.01</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>6.67</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>41.52</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>5.15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>2.59</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>4.59</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
-        <v>4.3600000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>4.36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>1.57</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>5.01</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>5.58</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>5.65</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>5.36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>1.82</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>2.13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>0.54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>6.3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>0.91</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>3.96</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>2.39</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>5.76</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>1.27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>2.94</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>3.73</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>3.01</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32">
-        <v>2.5299999999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>2.53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>6.59</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <v>5.43</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <v>3.89</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>2.83</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37">
-        <v>2.0499999999999998</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>2.05</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B38">
-        <v>2.2400000000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <v>2.24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="2">
         <v>1.07</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>5.49</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="2">
         <v>1.18</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <v>1.84</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="2">
         <v>1.44</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="2">
         <v>0.46</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="2">
         <v>2.61</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="2">
         <v>3.19</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="2">
         <v>3.73</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="2">
         <v>1.75</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="2">
         <v>3.22</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="2">
         <v>1.74</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B52">
-        <v>4.5199999999999996</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
+        <v>4.52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="2">
         <v>3.07</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="2">
         <v>4.5</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="2">
         <v>2.09</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="2">
         <v>3.48</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="2">
         <v>4.3</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="2">
         <v>2.02</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="2">
         <v>2.73</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="2">
         <v>5.75</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="2">
         <v>3.26</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="2">
         <v>1.59</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="2">
         <v>9.82</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="2">
         <v>3.02</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="2">
         <v>2.12</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="2">
         <v>2.21</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="2">
         <v>0.78</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B68">
-        <v>1.1299999999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="2">
+        <v>1.13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="2">
         <v>2.1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="2">
         <v>1.93</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="2">
         <v>5.96</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="2">
         <v>1.89</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="2">
         <v>6.95</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="2">
         <v>3.84</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B76">
-        <v>1.0900000000000001</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="2">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B77">
-        <v>4.6500000000000004</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="2">
+        <v>4.65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="2">
         <v>5.6</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B79">
-        <v>2.5299999999999998</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="2">
+        <v>2.53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="2">
         <v>1.91</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2">
       <c r="A81" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="2">
         <v>5.89</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="2">
         <v>5.77</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2">
       <c r="A83" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="2">
         <v>8.24</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="2">
         <v>0.59</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="2">
         <v>0.83</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2">
       <c r="A86" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="2">
         <v>5.96</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="2">
         <v>5.27</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="2">
         <v>3.71</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2">
       <c r="A89" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="2">
         <v>1.66</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2">
       <c r="A90" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="2">
         <v>2.77</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2">
       <c r="A91" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="2">
         <v>5.49</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2">
       <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="2">
         <v>5.35</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2">
       <c r="A93" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="2">
         <v>3.61</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2">
       <c r="A94" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="2">
         <v>3.38</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2">
       <c r="A95" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="2">
         <v>2.52</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2">
       <c r="A96" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="2">
         <v>1.79</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2">
       <c r="A97" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="2">
         <v>4.22</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="2">
         <v>2.9</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2">
       <c r="A99" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="2">
         <v>3.63</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2">
       <c r="A100" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="2">
         <v>1.01</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2">
       <c r="A101" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="2">
         <v>1.55</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2">
       <c r="A102" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="2">
         <v>4.58</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2">
       <c r="A103" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="2">
         <v>2.14</v>
       </c>
     </row>

</xml_diff>